<commit_message>
- added reference to maryland metrics: They have better and more info on   threads than amesweb.
</commit_message>
<xml_diff>
--- a/threads.xlsx
+++ b/threads.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian/Projects/Waterrockets/Bottle2GardenaAdapterWithFins/BSPthread/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian/Documents/OpenSCAD/libraries/threadlib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E46F0898-C66F-4341-9A5F-FF07F515C0EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F1AAB6-E67F-B04C-A39E-473D0299A0AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19800" yWindow="460" windowWidth="18600" windowHeight="21140" activeTab="1" xr2:uid="{46C58C85-D7E3-B144-AD74-40B7546B4D31}"/>
+    <workbookView xWindow="19800" yWindow="460" windowWidth="18600" windowHeight="21140" xr2:uid="{46C58C85-D7E3-B144-AD74-40B7546B4D31}"/>
   </bookViews>
   <sheets>
     <sheet name="BSPP thread" sheetId="1" r:id="rId1"/>
@@ -981,33 +981,6 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
@@ -1038,7 +1011,45 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1047,17 +1058,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1080,12 +1080,12 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5047857" cy="436786"/>
+    <xdr:ext cx="5047857" cy="953466"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="TextBox 1">
@@ -1099,8 +1099,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1333500" y="6667500"/>
-          <a:ext cx="5047857" cy="436786"/>
+          <a:off x="1143000" y="6654800"/>
+          <a:ext cx="5047857" cy="953466"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1138,6 +1138,25 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
             <a:t>https://www.amesweb.info/Screws/British-Standard-Pipe-Parallel-Thread-BSPP.aspx</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Even better info</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> (also on other thread types) here:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>http://mdmetric.com/tech/thddat7.htm</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1568,9 +1587,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4410726-507D-0E4E-8A5F-51222B2316ED}">
   <dimension ref="A1:Y28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C3" sqref="C3"/>
+      <selection pane="topRight" activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1602,43 +1621,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="17" thickBot="1">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="61" t="s">
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="62"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="62" t="s">
+      <c r="F1" s="100"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="62"/>
-      <c r="J1" s="61" t="s">
+      <c r="I1" s="100"/>
+      <c r="J1" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="63"/>
+      <c r="K1" s="101"/>
       <c r="L1" s="17"/>
-      <c r="M1" s="58" t="s">
+      <c r="M1" s="96" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="60"/>
+      <c r="N1" s="97"/>
+      <c r="O1" s="97"/>
+      <c r="P1" s="97"/>
+      <c r="Q1" s="98"/>
       <c r="R1" s="54">
         <v>0.27205047575333813</v>
       </c>
-      <c r="T1" s="58" t="s">
+      <c r="T1" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="60"/>
+      <c r="U1" s="97"/>
+      <c r="V1" s="97"/>
+      <c r="W1" s="97"/>
+      <c r="X1" s="98"/>
       <c r="Y1" s="54">
         <v>0.29097758142887981</v>
       </c>
@@ -3813,8 +3832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD97861-A178-2F47-B44F-F4D36A633F45}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3826,2457 +3845,2457 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17" thickBot="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="95" t="s">
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="104" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="96"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="105"/>
     </row>
     <row r="2" spans="1:12" s="10" customFormat="1" ht="17" thickBot="1">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="81" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="84" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="97" t="s">
+      <c r="E2" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="92" t="s">
+      <c r="F2" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="92" t="s">
+      <c r="G2" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="92" t="s">
+      <c r="H2" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="92" t="s">
+      <c r="I2" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="92" t="s">
+      <c r="J2" s="83" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="92" t="s">
+      <c r="K2" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="93" t="s">
+      <c r="L2" s="84" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="73" t="str">
+      <c r="A3" s="64" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A3,"-int")</f>
         <v>G1/16-int</v>
       </c>
-      <c r="B3" s="105">
+      <c r="B3" s="92">
         <f>'BSPP thread'!C3</f>
         <v>0.90700000000000003</v>
       </c>
-      <c r="C3" s="100">
+      <c r="C3" s="87">
         <f>'BSPP thread'!$M3/2+5*$B3/(24*TAN(phi/2))*1.05</f>
         <v>3.9788848601293729</v>
       </c>
-      <c r="D3" s="99">
+      <c r="D3" s="86">
         <f>'BSPP thread'!$M3+5*$B3/(12*TAN(phi/2))</f>
         <v>7.9214711621511862</v>
       </c>
-      <c r="E3" s="77">
+      <c r="E3" s="68">
         <f>'BSPP thread'!$M3/2+5*$B3/(24*TAN(phi/2))*1.05-C3</f>
         <v>0</v>
       </c>
-      <c r="F3" s="78">
+      <c r="F3" s="69">
         <f>0.46875*$B3</f>
         <v>0.42515625000000001</v>
       </c>
-      <c r="G3" s="78">
+      <c r="G3" s="69">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="H3" s="78">
+      <c r="H3" s="69">
         <f>-F3</f>
         <v>-0.42515625000000001</v>
       </c>
-      <c r="I3" s="78">
+      <c r="I3" s="69">
         <f>'BSPP thread'!$M3/2-$B3*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C3</f>
         <v>-0.56084140616326339</v>
       </c>
-      <c r="J3" s="78">
+      <c r="J3" s="69">
         <f>-0.13701*$B3</f>
         <v>-0.12426806999999999</v>
       </c>
-      <c r="K3" s="78">
+      <c r="K3" s="69">
         <f>I3</f>
         <v>-0.56084140616326339</v>
       </c>
-      <c r="L3" s="79">
+      <c r="L3" s="70">
         <f>-J3</f>
         <v>0.12426806999999999</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="74" t="str">
+      <c r="A4" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A4,"-int")</f>
         <v>G1/8-int</v>
       </c>
-      <c r="B4" s="68">
+      <c r="B4" s="59">
         <f>'BSPP thread'!C4</f>
         <v>0.90700000000000003</v>
       </c>
-      <c r="C4" s="101">
+      <c r="C4" s="88">
         <f>'BSPP thread'!$M4/2+5*$B4/(24*TAN(phi/2))*1.05</f>
         <v>4.9813848601293724</v>
       </c>
-      <c r="D4" s="76">
+      <c r="D4" s="67">
         <f>'BSPP thread'!$M4+5*$B4/(12*TAN(phi/2))</f>
         <v>9.9264711621511861</v>
       </c>
-      <c r="E4" s="68">
+      <c r="E4" s="59">
         <f>'BSPP thread'!$M4/2+5*$B4/(24*TAN(phi/2))*1.05-C4</f>
         <v>0</v>
       </c>
-      <c r="F4" s="64">
+      <c r="F4" s="55">
         <f t="shared" ref="F4:F26" si="0">0.46875*$B4</f>
         <v>0.42515625000000001</v>
       </c>
-      <c r="G4" s="64">
+      <c r="G4" s="55">
         <f t="shared" ref="G4:G26" si="1">E4</f>
         <v>0</v>
       </c>
-      <c r="H4" s="64">
+      <c r="H4" s="55">
         <f t="shared" ref="H4:H26" si="2">-F4</f>
         <v>-0.42515625000000001</v>
       </c>
-      <c r="I4" s="64">
+      <c r="I4" s="55">
         <f>'BSPP thread'!$M4/2-$B4*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C4</f>
         <v>-0.56084140616326295</v>
       </c>
-      <c r="J4" s="64">
+      <c r="J4" s="55">
         <f t="shared" ref="J4:J26" si="3">-0.13701*$B4</f>
         <v>-0.12426806999999999</v>
       </c>
-      <c r="K4" s="64">
+      <c r="K4" s="55">
         <f t="shared" ref="K4:K26" si="4">I4</f>
         <v>-0.56084140616326295</v>
       </c>
-      <c r="L4" s="69">
+      <c r="L4" s="60">
         <f t="shared" ref="L4:L26" si="5">-J4</f>
         <v>0.12426806999999999</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="74" t="str">
+      <c r="A5" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A5,"-int")</f>
         <v>G1/4-int</v>
       </c>
-      <c r="B5" s="68">
+      <c r="B5" s="59">
         <f>'BSPP thread'!C5</f>
         <v>1.337</v>
       </c>
-      <c r="C5" s="101">
+      <c r="C5" s="88">
         <f>'BSPP thread'!$M5/2+5*$B5/(24*TAN(phi/2))*1.05</f>
         <v>6.7435772414475981</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="67">
         <f>'BSPP thread'!$M5+5*$B5/(12*TAN(phi/2))</f>
         <v>13.433647126566854</v>
       </c>
-      <c r="E5" s="68">
+      <c r="E5" s="59">
         <f>'BSPP thread'!$M5/2+5*$B5/(24*TAN(phi/2))*1.05-C5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="64">
+      <c r="F5" s="55">
         <f t="shared" si="0"/>
         <v>0.62671874999999999</v>
       </c>
-      <c r="G5" s="64">
+      <c r="G5" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H5" s="64">
+      <c r="H5" s="55">
         <f t="shared" si="2"/>
         <v>-0.62671874999999999</v>
       </c>
-      <c r="I5" s="64">
+      <c r="I5" s="55">
         <f>'BSPP thread'!$M5/2-$B5*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C5</f>
         <v>-0.82673093719987101</v>
       </c>
-      <c r="J5" s="64">
+      <c r="J5" s="55">
         <f t="shared" si="3"/>
         <v>-0.18318236999999998</v>
       </c>
-      <c r="K5" s="64">
+      <c r="K5" s="55">
         <f t="shared" si="4"/>
         <v>-0.82673093719987101</v>
       </c>
-      <c r="L5" s="69">
+      <c r="L5" s="60">
         <f t="shared" si="5"/>
         <v>0.18318236999999998</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="74" t="str">
+      <c r="A6" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A6,"-int")</f>
         <v>G3/8-int</v>
       </c>
-      <c r="B6" s="68">
+      <c r="B6" s="59">
         <f>'BSPP thread'!C6</f>
         <v>1.337</v>
       </c>
-      <c r="C6" s="101">
+      <c r="C6" s="88">
         <f>'BSPP thread'!$M6/2+5*$B6/(24*TAN(phi/2))*1.05</f>
         <v>8.4960772414475976</v>
       </c>
-      <c r="D6" s="76">
+      <c r="D6" s="67">
         <f>'BSPP thread'!$M6+5*$B6/(12*TAN(phi/2))</f>
         <v>16.938647126566853</v>
       </c>
-      <c r="E6" s="68">
+      <c r="E6" s="59">
         <f>'BSPP thread'!$M6/2+5*$B6/(24*TAN(phi/2))*1.05-C6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="64">
+      <c r="F6" s="55">
         <f t="shared" si="0"/>
         <v>0.62671874999999999</v>
       </c>
-      <c r="G6" s="64">
+      <c r="G6" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H6" s="64">
+      <c r="H6" s="55">
         <f t="shared" si="2"/>
         <v>-0.62671874999999999</v>
       </c>
-      <c r="I6" s="64">
+      <c r="I6" s="55">
         <f>'BSPP thread'!$M6/2-$B6*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C6</f>
         <v>-0.82673093719987101</v>
       </c>
-      <c r="J6" s="64">
+      <c r="J6" s="55">
         <f t="shared" si="3"/>
         <v>-0.18318236999999998</v>
       </c>
-      <c r="K6" s="64">
+      <c r="K6" s="55">
         <f t="shared" si="4"/>
         <v>-0.82673093719987101</v>
       </c>
-      <c r="L6" s="69">
+      <c r="L6" s="60">
         <f t="shared" si="5"/>
         <v>0.18318236999999998</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="74" t="str">
+      <c r="A7" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A7,"-int")</f>
         <v>G1/2-int</v>
       </c>
-      <c r="B7" s="68">
+      <c r="B7" s="59">
         <f>'BSPP thread'!C7</f>
         <v>1.8140000000000001</v>
       </c>
-      <c r="C7" s="101">
+      <c r="C7" s="88">
         <f>'BSPP thread'!$M7/2+5*$B7/(24*TAN(phi/2))*1.05</f>
         <v>10.694269720258745</v>
       </c>
-      <c r="D7" s="76">
+      <c r="D7" s="67">
         <f>'BSPP thread'!$M7+5*$B7/(12*TAN(phi/2))</f>
         <v>21.315942324302373</v>
       </c>
-      <c r="E7" s="68">
+      <c r="E7" s="59">
         <f>'BSPP thread'!$M7/2+5*$B7/(24*TAN(phi/2))*1.05-C7</f>
         <v>0</v>
       </c>
-      <c r="F7" s="64">
+      <c r="F7" s="55">
         <f t="shared" si="0"/>
         <v>0.85031250000000003</v>
       </c>
-      <c r="G7" s="64">
+      <c r="G7" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H7" s="64">
+      <c r="H7" s="55">
         <f t="shared" si="2"/>
         <v>-0.85031250000000003</v>
       </c>
-      <c r="I7" s="64">
+      <c r="I7" s="55">
         <f>'BSPP thread'!$M7/2-$B7*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C7</f>
         <v>-1.1216828123265259</v>
       </c>
-      <c r="J7" s="64">
+      <c r="J7" s="55">
         <f t="shared" si="3"/>
         <v>-0.24853613999999999</v>
       </c>
-      <c r="K7" s="64">
+      <c r="K7" s="55">
         <f t="shared" si="4"/>
         <v>-1.1216828123265259</v>
       </c>
-      <c r="L7" s="69">
+      <c r="L7" s="60">
         <f t="shared" si="5"/>
         <v>0.24853613999999999</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="74" t="str">
+      <c r="A8" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A8,"-int")</f>
         <v>G5/8-int</v>
       </c>
-      <c r="B8" s="68">
+      <c r="B8" s="59">
         <f>'BSPP thread'!C8</f>
         <v>1.8140000000000001</v>
       </c>
-      <c r="C8" s="101">
+      <c r="C8" s="88">
         <f>'BSPP thread'!$M8/2+5*$B8/(24*TAN(phi/2))*1.05</f>
         <v>11.672269720258747</v>
       </c>
-      <c r="D8" s="76">
+      <c r="D8" s="67">
         <f>'BSPP thread'!$M8+5*$B8/(12*TAN(phi/2))</f>
         <v>23.271942324302373</v>
       </c>
-      <c r="E8" s="68">
+      <c r="E8" s="59">
         <f>'BSPP thread'!$M8/2+5*$B8/(24*TAN(phi/2))*1.05-C8</f>
         <v>0</v>
       </c>
-      <c r="F8" s="64">
+      <c r="F8" s="55">
         <f t="shared" si="0"/>
         <v>0.85031250000000003</v>
       </c>
-      <c r="G8" s="64">
+      <c r="G8" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H8" s="64">
+      <c r="H8" s="55">
         <f t="shared" si="2"/>
         <v>-0.85031250000000003</v>
       </c>
-      <c r="I8" s="64">
+      <c r="I8" s="55">
         <f>'BSPP thread'!$M8/2-$B8*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C8</f>
         <v>-1.1216828123265277</v>
       </c>
-      <c r="J8" s="64">
+      <c r="J8" s="55">
         <f t="shared" si="3"/>
         <v>-0.24853613999999999</v>
       </c>
-      <c r="K8" s="64">
+      <c r="K8" s="55">
         <f t="shared" si="4"/>
         <v>-1.1216828123265277</v>
       </c>
-      <c r="L8" s="69">
+      <c r="L8" s="60">
         <f t="shared" si="5"/>
         <v>0.24853613999999999</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="74" t="str">
+      <c r="A9" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A9,"-int")</f>
         <v>G3/4-int</v>
       </c>
-      <c r="B9" s="68">
+      <c r="B9" s="59">
         <f>'BSPP thread'!C9</f>
         <v>1.8140000000000001</v>
       </c>
-      <c r="C9" s="101">
+      <c r="C9" s="88">
         <f>'BSPP thread'!$M9/2+5*$B9/(24*TAN(phi/2))*1.05</f>
         <v>13.437269720258747</v>
       </c>
-      <c r="D9" s="76">
+      <c r="D9" s="67">
         <f>'BSPP thread'!$M9+5*$B9/(12*TAN(phi/2))</f>
         <v>26.801942324302374</v>
       </c>
-      <c r="E9" s="68">
+      <c r="E9" s="59">
         <f>'BSPP thread'!$M9/2+5*$B9/(24*TAN(phi/2))*1.05-C9</f>
         <v>0</v>
       </c>
-      <c r="F9" s="64">
+      <c r="F9" s="55">
         <f t="shared" si="0"/>
         <v>0.85031250000000003</v>
       </c>
-      <c r="G9" s="64">
+      <c r="G9" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H9" s="64">
+      <c r="H9" s="55">
         <f t="shared" si="2"/>
         <v>-0.85031250000000003</v>
       </c>
-      <c r="I9" s="64">
+      <c r="I9" s="55">
         <f>'BSPP thread'!$M9/2-$B9*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C9</f>
         <v>-1.1216828123265277</v>
       </c>
-      <c r="J9" s="64">
+      <c r="J9" s="55">
         <f t="shared" si="3"/>
         <v>-0.24853613999999999</v>
       </c>
-      <c r="K9" s="64">
+      <c r="K9" s="55">
         <f t="shared" si="4"/>
         <v>-1.1216828123265277</v>
       </c>
-      <c r="L9" s="69">
+      <c r="L9" s="60">
         <f t="shared" si="5"/>
         <v>0.24853613999999999</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="74" t="str">
+      <c r="A10" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A10,"-int")</f>
         <v>G7/8-int</v>
       </c>
-      <c r="B10" s="68">
+      <c r="B10" s="59">
         <f>'BSPP thread'!C10</f>
         <v>1.8140000000000001</v>
       </c>
-      <c r="C10" s="101">
+      <c r="C10" s="88">
         <f>'BSPP thread'!$M10/2+5*$B10/(24*TAN(phi/2))*1.05</f>
         <v>15.317269720258746</v>
       </c>
-      <c r="D10" s="76">
+      <c r="D10" s="67">
         <f>'BSPP thread'!$M10+5*$B10/(12*TAN(phi/2))</f>
         <v>30.561942324302375</v>
       </c>
-      <c r="E10" s="68">
+      <c r="E10" s="59">
         <f>'BSPP thread'!$M10/2+5*$B10/(24*TAN(phi/2))*1.05-C10</f>
         <v>0</v>
       </c>
-      <c r="F10" s="64">
+      <c r="F10" s="55">
         <f t="shared" si="0"/>
         <v>0.85031250000000003</v>
       </c>
-      <c r="G10" s="64">
+      <c r="G10" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H10" s="64">
+      <c r="H10" s="55">
         <f t="shared" si="2"/>
         <v>-0.85031250000000003</v>
       </c>
-      <c r="I10" s="64">
+      <c r="I10" s="55">
         <f>'BSPP thread'!$M10/2-$B10*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C10</f>
         <v>-1.1216828123265259</v>
       </c>
-      <c r="J10" s="64">
+      <c r="J10" s="55">
         <f t="shared" si="3"/>
         <v>-0.24853613999999999</v>
       </c>
-      <c r="K10" s="64">
+      <c r="K10" s="55">
         <f t="shared" si="4"/>
         <v>-1.1216828123265259</v>
       </c>
-      <c r="L10" s="69">
+      <c r="L10" s="60">
         <f t="shared" si="5"/>
         <v>0.24853613999999999</v>
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="74" t="str">
+      <c r="A11" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A11,"-int")</f>
         <v>G1-int</v>
       </c>
-      <c r="B11" s="68">
+      <c r="B11" s="59">
         <f>'BSPP thread'!C11</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C11" s="101">
+      <c r="C11" s="88">
         <f>'BSPP thread'!$M11/2+5*$B11/(24*TAN(phi/2))*1.05</f>
         <v>16.900276066194841</v>
       </c>
-      <c r="D11" s="76">
+      <c r="D11" s="67">
         <f>'BSPP thread'!$M11+5*$B11/(12*TAN(phi/2))</f>
         <v>33.708144887990173</v>
       </c>
-      <c r="E11" s="68">
+      <c r="E11" s="59">
         <f>'BSPP thread'!$M11/2+5*$B11/(24*TAN(phi/2))*1.05-C11</f>
         <v>0</v>
       </c>
-      <c r="F11" s="64">
+      <c r="F11" s="55">
         <f t="shared" si="0"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="G11" s="64">
+      <c r="G11" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H11" s="64">
+      <c r="H11" s="55">
         <f t="shared" si="2"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="I11" s="64">
+      <c r="I11" s="55">
         <f>'BSPP thread'!$M11/2-$B11*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C11</f>
         <v>-1.4277649468919229</v>
       </c>
-      <c r="J11" s="64">
+      <c r="J11" s="55">
         <f t="shared" si="3"/>
         <v>-0.31635608999999998</v>
       </c>
-      <c r="K11" s="64">
+      <c r="K11" s="55">
         <f t="shared" si="4"/>
         <v>-1.4277649468919229</v>
       </c>
-      <c r="L11" s="69">
+      <c r="L11" s="60">
         <f t="shared" si="5"/>
         <v>0.31635608999999998</v>
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="74" t="str">
+      <c r="A12" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A12,"-int")</f>
         <v>G1 1/8-int</v>
       </c>
-      <c r="B12" s="68">
+      <c r="B12" s="59">
         <f>'BSPP thread'!C12</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C12" s="101">
+      <c r="C12" s="88">
         <f>'BSPP thread'!$M12/2+5*$B12/(24*TAN(phi/2))*1.05</f>
         <v>19.224276066194843</v>
       </c>
-      <c r="D12" s="76">
+      <c r="D12" s="67">
         <f>'BSPP thread'!$M12+5*$B12/(12*TAN(phi/2))</f>
         <v>38.356144887990176</v>
       </c>
-      <c r="E12" s="68">
+      <c r="E12" s="59">
         <f>'BSPP thread'!$M12/2+5*$B12/(24*TAN(phi/2))*1.05-C12</f>
         <v>0</v>
       </c>
-      <c r="F12" s="64">
+      <c r="F12" s="55">
         <f t="shared" si="0"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="G12" s="64">
+      <c r="G12" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H12" s="64">
+      <c r="H12" s="55">
         <f t="shared" si="2"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="I12" s="64">
+      <c r="I12" s="55">
         <f>'BSPP thread'!$M12/2-$B12*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C12</f>
         <v>-1.4277649468919229</v>
       </c>
-      <c r="J12" s="64">
+      <c r="J12" s="55">
         <f t="shared" si="3"/>
         <v>-0.31635608999999998</v>
       </c>
-      <c r="K12" s="64">
+      <c r="K12" s="55">
         <f t="shared" si="4"/>
         <v>-1.4277649468919229</v>
       </c>
-      <c r="L12" s="69">
+      <c r="L12" s="60">
         <f t="shared" si="5"/>
         <v>0.31635608999999998</v>
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="74" t="str">
+      <c r="A13" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A13,"-int")</f>
         <v>G1 1/4-int</v>
       </c>
-      <c r="B13" s="68">
+      <c r="B13" s="59">
         <f>'BSPP thread'!C13</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C13" s="101">
+      <c r="C13" s="88">
         <f>'BSPP thread'!$M13/2+5*$B13/(24*TAN(phi/2))*1.05</f>
         <v>21.230776066194842</v>
       </c>
-      <c r="D13" s="76">
+      <c r="D13" s="67">
         <f>'BSPP thread'!$M13+5*$B13/(12*TAN(phi/2))</f>
         <v>42.369144887990174</v>
       </c>
-      <c r="E13" s="68">
+      <c r="E13" s="59">
         <f>'BSPP thread'!$M13/2+5*$B13/(24*TAN(phi/2))*1.05-C13</f>
         <v>0</v>
       </c>
-      <c r="F13" s="64">
+      <c r="F13" s="55">
         <f t="shared" si="0"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="G13" s="64">
+      <c r="G13" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H13" s="64">
+      <c r="H13" s="55">
         <f t="shared" si="2"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="I13" s="64">
+      <c r="I13" s="55">
         <f>'BSPP thread'!$M13/2-$B13*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C13</f>
         <v>-1.4277649468919229</v>
       </c>
-      <c r="J13" s="64">
+      <c r="J13" s="55">
         <f t="shared" si="3"/>
         <v>-0.31635608999999998</v>
       </c>
-      <c r="K13" s="64">
+      <c r="K13" s="55">
         <f t="shared" si="4"/>
         <v>-1.4277649468919229</v>
       </c>
-      <c r="L13" s="69">
+      <c r="L13" s="60">
         <f t="shared" si="5"/>
         <v>0.31635608999999998</v>
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="74" t="str">
+      <c r="A14" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A14,"-int")</f>
         <v>G1 1/2-int</v>
       </c>
-      <c r="B14" s="68">
+      <c r="B14" s="59">
         <f>'BSPP thread'!C14</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C14" s="101">
+      <c r="C14" s="88">
         <f>'BSPP thread'!$M14/2+5*$B14/(24*TAN(phi/2))*1.05</f>
         <v>24.177276066194842</v>
       </c>
-      <c r="D14" s="76">
+      <c r="D14" s="67">
         <f>'BSPP thread'!$M14+5*$B14/(12*TAN(phi/2))</f>
         <v>48.262144887990175</v>
       </c>
-      <c r="E14" s="68">
+      <c r="E14" s="59">
         <f>'BSPP thread'!$M14/2+5*$B14/(24*TAN(phi/2))*1.05-C14</f>
         <v>0</v>
       </c>
-      <c r="F14" s="64">
+      <c r="F14" s="55">
         <f t="shared" si="0"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="G14" s="64">
+      <c r="G14" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H14" s="64">
+      <c r="H14" s="55">
         <f t="shared" si="2"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="I14" s="64">
+      <c r="I14" s="55">
         <f>'BSPP thread'!$M14/2-$B14*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C14</f>
         <v>-1.4277649468919229</v>
       </c>
-      <c r="J14" s="64">
+      <c r="J14" s="55">
         <f t="shared" si="3"/>
         <v>-0.31635608999999998</v>
       </c>
-      <c r="K14" s="64">
+      <c r="K14" s="55">
         <f t="shared" si="4"/>
         <v>-1.4277649468919229</v>
       </c>
-      <c r="L14" s="69">
+      <c r="L14" s="60">
         <f t="shared" si="5"/>
         <v>0.31635608999999998</v>
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="74" t="str">
+      <c r="A15" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A15,"-int")</f>
         <v>G1 3/4-int</v>
       </c>
-      <c r="B15" s="68">
+      <c r="B15" s="59">
         <f>'BSPP thread'!C15</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C15" s="101">
+      <c r="C15" s="88">
         <f>'BSPP thread'!$M15/2+5*$B15/(24*TAN(phi/2))*1.05</f>
         <v>27.148776066194845</v>
       </c>
-      <c r="D15" s="76">
+      <c r="D15" s="67">
         <f>'BSPP thread'!$M15+5*$B15/(12*TAN(phi/2))</f>
         <v>54.20514488799018</v>
       </c>
-      <c r="E15" s="68">
+      <c r="E15" s="59">
         <f>'BSPP thread'!$M15/2+5*$B15/(24*TAN(phi/2))*1.05-C15</f>
         <v>0</v>
       </c>
-      <c r="F15" s="64">
+      <c r="F15" s="55">
         <f t="shared" si="0"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="G15" s="64">
+      <c r="G15" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H15" s="64">
+      <c r="H15" s="55">
         <f t="shared" si="2"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="I15" s="64">
+      <c r="I15" s="55">
         <f>'BSPP thread'!$M15/2-$B15*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C15</f>
         <v>-1.4277649468919229</v>
       </c>
-      <c r="J15" s="64">
+      <c r="J15" s="55">
         <f t="shared" si="3"/>
         <v>-0.31635608999999998</v>
       </c>
-      <c r="K15" s="64">
+      <c r="K15" s="55">
         <f t="shared" si="4"/>
         <v>-1.4277649468919229</v>
       </c>
-      <c r="L15" s="69">
+      <c r="L15" s="60">
         <f t="shared" si="5"/>
         <v>0.31635608999999998</v>
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="74" t="str">
+      <c r="A16" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A16,"-int")</f>
         <v>G2-int</v>
       </c>
-      <c r="B16" s="68">
+      <c r="B16" s="59">
         <f>'BSPP thread'!C16</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C16" s="101">
+      <c r="C16" s="88">
         <f>'BSPP thread'!$M16/2+5*$B16/(24*TAN(phi/2))*1.05</f>
         <v>30.082776066194842</v>
       </c>
-      <c r="D16" s="76">
+      <c r="D16" s="67">
         <f>'BSPP thread'!$M16+5*$B16/(12*TAN(phi/2))</f>
         <v>60.073144887990175</v>
       </c>
-      <c r="E16" s="68">
+      <c r="E16" s="59">
         <f>'BSPP thread'!$M16/2+5*$B16/(24*TAN(phi/2))*1.05-C16</f>
         <v>0</v>
       </c>
-      <c r="F16" s="64">
+      <c r="F16" s="55">
         <f t="shared" si="0"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="G16" s="64">
+      <c r="G16" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H16" s="64">
+      <c r="H16" s="55">
         <f t="shared" si="2"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="I16" s="64">
+      <c r="I16" s="55">
         <f>'BSPP thread'!$M16/2-$B16*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C16</f>
         <v>-1.4277649468919229</v>
       </c>
-      <c r="J16" s="64">
+      <c r="J16" s="55">
         <f t="shared" si="3"/>
         <v>-0.31635608999999998</v>
       </c>
-      <c r="K16" s="64">
+      <c r="K16" s="55">
         <f t="shared" si="4"/>
         <v>-1.4277649468919229</v>
       </c>
-      <c r="L16" s="69">
+      <c r="L16" s="60">
         <f t="shared" si="5"/>
         <v>0.31635608999999998</v>
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="74" t="str">
+      <c r="A17" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A17,"-int")</f>
         <v>G2 1/4-int</v>
       </c>
-      <c r="B17" s="68">
+      <c r="B17" s="59">
         <f>'BSPP thread'!C17</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C17" s="101">
+      <c r="C17" s="88">
         <f>'BSPP thread'!$M17/2+5*$B17/(24*TAN(phi/2))*1.05</f>
         <v>33.140026066194842</v>
       </c>
-      <c r="D17" s="76">
+      <c r="D17" s="67">
         <f>'BSPP thread'!$M17+5*$B17/(12*TAN(phi/2))</f>
         <v>66.187644887990174</v>
       </c>
-      <c r="E17" s="68">
+      <c r="E17" s="59">
         <f>'BSPP thread'!$M17/2+5*$B17/(24*TAN(phi/2))*1.05-C17</f>
         <v>0</v>
       </c>
-      <c r="F17" s="64">
+      <c r="F17" s="55">
         <f t="shared" si="0"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="G17" s="64">
+      <c r="G17" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H17" s="64">
+      <c r="H17" s="55">
         <f t="shared" si="2"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="I17" s="64">
+      <c r="I17" s="55">
         <f>'BSPP thread'!$M17/2-$B17*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C17</f>
         <v>-1.4277649468919229</v>
       </c>
-      <c r="J17" s="64">
+      <c r="J17" s="55">
         <f t="shared" si="3"/>
         <v>-0.31635608999999998</v>
       </c>
-      <c r="K17" s="64">
+      <c r="K17" s="55">
         <f t="shared" si="4"/>
         <v>-1.4277649468919229</v>
       </c>
-      <c r="L17" s="69">
+      <c r="L17" s="60">
         <f t="shared" si="5"/>
         <v>0.31635608999999998</v>
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="74" t="str">
+      <c r="A18" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A18,"-int")</f>
         <v>G2 1/2-int</v>
       </c>
-      <c r="B18" s="68">
+      <c r="B18" s="59">
         <f>'BSPP thread'!C18</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C18" s="101">
+      <c r="C18" s="88">
         <f>'BSPP thread'!$M18/2+5*$B18/(24*TAN(phi/2))*1.05</f>
         <v>37.877026066194844</v>
       </c>
-      <c r="D18" s="76">
+      <c r="D18" s="67">
         <f>'BSPP thread'!$M18+5*$B18/(12*TAN(phi/2))</f>
         <v>75.661644887990178</v>
       </c>
-      <c r="E18" s="68">
+      <c r="E18" s="59">
         <f>'BSPP thread'!$M18/2+5*$B18/(24*TAN(phi/2))*1.05-C18</f>
         <v>0</v>
       </c>
-      <c r="F18" s="64">
+      <c r="F18" s="55">
         <f t="shared" si="0"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="G18" s="64">
+      <c r="G18" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H18" s="64">
+      <c r="H18" s="55">
         <f t="shared" si="2"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="I18" s="64">
+      <c r="I18" s="55">
         <f>'BSPP thread'!$M18/2-$B18*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C18</f>
         <v>-1.4277649468919265</v>
       </c>
-      <c r="J18" s="64">
+      <c r="J18" s="55">
         <f t="shared" si="3"/>
         <v>-0.31635608999999998</v>
       </c>
-      <c r="K18" s="64">
+      <c r="K18" s="55">
         <f t="shared" si="4"/>
         <v>-1.4277649468919265</v>
       </c>
-      <c r="L18" s="69">
+      <c r="L18" s="60">
         <f t="shared" si="5"/>
         <v>0.31635608999999998</v>
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="74" t="str">
+      <c r="A19" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A19,"-int")</f>
         <v>G2 3/4-int</v>
       </c>
-      <c r="B19" s="68">
+      <c r="B19" s="59">
         <f>'BSPP thread'!C19</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C19" s="101">
+      <c r="C19" s="88">
         <f>'BSPP thread'!$M19/2+5*$B19/(24*TAN(phi/2))*1.05</f>
         <v>41.052026066194848</v>
       </c>
-      <c r="D19" s="76">
+      <c r="D19" s="67">
         <f>'BSPP thread'!$M19+5*$B19/(12*TAN(phi/2))</f>
         <v>82.011644887990187</v>
       </c>
-      <c r="E19" s="68">
+      <c r="E19" s="59">
         <f>'BSPP thread'!$M19/2+5*$B19/(24*TAN(phi/2))*1.05-C19</f>
         <v>0</v>
       </c>
-      <c r="F19" s="64">
+      <c r="F19" s="55">
         <f t="shared" si="0"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="G19" s="64">
+      <c r="G19" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H19" s="64">
+      <c r="H19" s="55">
         <f t="shared" si="2"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="I19" s="64">
+      <c r="I19" s="55">
         <f>'BSPP thread'!$M19/2-$B19*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C19</f>
         <v>-1.4277649468919265</v>
       </c>
-      <c r="J19" s="64">
+      <c r="J19" s="55">
         <f t="shared" si="3"/>
         <v>-0.31635608999999998</v>
       </c>
-      <c r="K19" s="64">
+      <c r="K19" s="55">
         <f t="shared" si="4"/>
         <v>-1.4277649468919265</v>
       </c>
-      <c r="L19" s="69">
+      <c r="L19" s="60">
         <f t="shared" si="5"/>
         <v>0.31635608999999998</v>
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="74" t="str">
+      <c r="A20" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A20,"-int")</f>
         <v>G3-int</v>
       </c>
-      <c r="B20" s="68">
+      <c r="B20" s="59">
         <f>'BSPP thread'!C20</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C20" s="101">
+      <c r="C20" s="88">
         <f>'BSPP thread'!$M20/2+5*$B20/(24*TAN(phi/2))*1.05</f>
         <v>44.227026066194846</v>
       </c>
-      <c r="D20" s="76">
+      <c r="D20" s="67">
         <f>'BSPP thread'!$M20+5*$B20/(12*TAN(phi/2))</f>
         <v>88.361644887990181</v>
       </c>
-      <c r="E20" s="68">
+      <c r="E20" s="59">
         <f>'BSPP thread'!$M20/2+5*$B20/(24*TAN(phi/2))*1.05-C20</f>
         <v>0</v>
       </c>
-      <c r="F20" s="64">
+      <c r="F20" s="55">
         <f t="shared" si="0"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="G20" s="64">
+      <c r="G20" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H20" s="64">
+      <c r="H20" s="55">
         <f t="shared" si="2"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="I20" s="64">
+      <c r="I20" s="55">
         <f>'BSPP thread'!$M20/2-$B20*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C20</f>
         <v>-1.4277649468919265</v>
       </c>
-      <c r="J20" s="64">
+      <c r="J20" s="55">
         <f t="shared" si="3"/>
         <v>-0.31635608999999998</v>
       </c>
-      <c r="K20" s="64">
+      <c r="K20" s="55">
         <f t="shared" si="4"/>
         <v>-1.4277649468919265</v>
       </c>
-      <c r="L20" s="69">
+      <c r="L20" s="60">
         <f t="shared" si="5"/>
         <v>0.31635608999999998</v>
       </c>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="74" t="str">
+      <c r="A21" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A21,"-int")</f>
         <v>G3 1/2-int</v>
       </c>
-      <c r="B21" s="68">
+      <c r="B21" s="59">
         <f>'BSPP thread'!C21</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C21" s="101">
+      <c r="C21" s="88">
         <f>'BSPP thread'!$M21/2+5*$B21/(24*TAN(phi/2))*1.05</f>
         <v>50.450026066194845</v>
       </c>
-      <c r="D21" s="76">
+      <c r="D21" s="67">
         <f>'BSPP thread'!$M21+5*$B21/(12*TAN(phi/2))</f>
         <v>100.80764488799018</v>
       </c>
-      <c r="E21" s="68">
+      <c r="E21" s="59">
         <f>'BSPP thread'!$M21/2+5*$B21/(24*TAN(phi/2))*1.05-C21</f>
         <v>0</v>
       </c>
-      <c r="F21" s="64">
+      <c r="F21" s="55">
         <f t="shared" si="0"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="G21" s="64">
+      <c r="G21" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H21" s="64">
+      <c r="H21" s="55">
         <f t="shared" si="2"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="I21" s="64">
+      <c r="I21" s="55">
         <f>'BSPP thread'!$M21/2-$B21*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C21</f>
         <v>-1.4277649468919265</v>
       </c>
-      <c r="J21" s="64">
+      <c r="J21" s="55">
         <f t="shared" si="3"/>
         <v>-0.31635608999999998</v>
       </c>
-      <c r="K21" s="64">
+      <c r="K21" s="55">
         <f t="shared" si="4"/>
         <v>-1.4277649468919265</v>
       </c>
-      <c r="L21" s="69">
+      <c r="L21" s="60">
         <f t="shared" si="5"/>
         <v>0.31635608999999998</v>
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="74" t="str">
+      <c r="A22" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A22,"-int")</f>
         <v>G4-int</v>
       </c>
-      <c r="B22" s="68">
+      <c r="B22" s="59">
         <f>'BSPP thread'!C22</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C22" s="101">
+      <c r="C22" s="88">
         <f>'BSPP thread'!$M22/2+5*$B22/(24*TAN(phi/2))*1.05</f>
         <v>56.800026066194846</v>
       </c>
-      <c r="D22" s="76">
+      <c r="D22" s="67">
         <f>'BSPP thread'!$M22+5*$B22/(12*TAN(phi/2))</f>
         <v>113.50764488799018</v>
       </c>
-      <c r="E22" s="68">
+      <c r="E22" s="59">
         <f>'BSPP thread'!$M22/2+5*$B22/(24*TAN(phi/2))*1.05-C22</f>
         <v>0</v>
       </c>
-      <c r="F22" s="64">
+      <c r="F22" s="55">
         <f t="shared" si="0"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="G22" s="64">
+      <c r="G22" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H22" s="64">
+      <c r="H22" s="55">
         <f t="shared" si="2"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="I22" s="64">
+      <c r="I22" s="55">
         <f>'BSPP thread'!$M22/2-$B22*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C22</f>
         <v>-1.4277649468919265</v>
       </c>
-      <c r="J22" s="64">
+      <c r="J22" s="55">
         <f t="shared" si="3"/>
         <v>-0.31635608999999998</v>
       </c>
-      <c r="K22" s="64">
+      <c r="K22" s="55">
         <f t="shared" si="4"/>
         <v>-1.4277649468919265</v>
       </c>
-      <c r="L22" s="69">
+      <c r="L22" s="60">
         <f t="shared" si="5"/>
         <v>0.31635608999999998</v>
       </c>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="74" t="str">
+      <c r="A23" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A23,"-int")</f>
         <v>G4 1/2-int</v>
       </c>
-      <c r="B23" s="68">
+      <c r="B23" s="59">
         <f>'BSPP thread'!C23</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C23" s="101">
+      <c r="C23" s="88">
         <f>'BSPP thread'!$M23/2+5*$B23/(24*TAN(phi/2))*1.05</f>
         <v>63.150026066194847</v>
       </c>
-      <c r="D23" s="76">
+      <c r="D23" s="67">
         <f>'BSPP thread'!$M23+5*$B23/(12*TAN(phi/2))</f>
         <v>126.20764488799018</v>
       </c>
-      <c r="E23" s="68">
+      <c r="E23" s="59">
         <f>'BSPP thread'!$M23/2+5*$B23/(24*TAN(phi/2))*1.05-C23</f>
         <v>0</v>
       </c>
-      <c r="F23" s="64">
+      <c r="F23" s="55">
         <f t="shared" si="0"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="G23" s="64">
+      <c r="G23" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H23" s="64">
+      <c r="H23" s="55">
         <f t="shared" si="2"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="I23" s="64">
+      <c r="I23" s="55">
         <f>'BSPP thread'!$M23/2-$B23*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C23</f>
         <v>-1.4277649468919265</v>
       </c>
-      <c r="J23" s="64">
+      <c r="J23" s="55">
         <f t="shared" si="3"/>
         <v>-0.31635608999999998</v>
       </c>
-      <c r="K23" s="64">
+      <c r="K23" s="55">
         <f t="shared" si="4"/>
         <v>-1.4277649468919265</v>
       </c>
-      <c r="L23" s="69">
+      <c r="L23" s="60">
         <f t="shared" si="5"/>
         <v>0.31635608999999998</v>
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="74" t="str">
+      <c r="A24" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A24,"-int")</f>
         <v>G5-int</v>
       </c>
-      <c r="B24" s="68">
+      <c r="B24" s="59">
         <f>'BSPP thread'!C24</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C24" s="101">
+      <c r="C24" s="88">
         <f>'BSPP thread'!$M24/2+5*$B24/(24*TAN(phi/2))*1.05</f>
         <v>69.500026066194835</v>
       </c>
-      <c r="D24" s="76">
+      <c r="D24" s="67">
         <f>'BSPP thread'!$M24+5*$B24/(12*TAN(phi/2))</f>
         <v>138.90764488799016</v>
       </c>
-      <c r="E24" s="68">
+      <c r="E24" s="59">
         <f>'BSPP thread'!$M24/2+5*$B24/(24*TAN(phi/2))*1.05-C24</f>
         <v>0</v>
       </c>
-      <c r="F24" s="64">
+      <c r="F24" s="55">
         <f t="shared" si="0"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="G24" s="64">
+      <c r="G24" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H24" s="64">
+      <c r="H24" s="55">
         <f t="shared" si="2"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="I24" s="64">
+      <c r="I24" s="55">
         <f>'BSPP thread'!$M24/2-$B24*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C24</f>
         <v>-1.4277649468919265</v>
       </c>
-      <c r="J24" s="64">
+      <c r="J24" s="55">
         <f t="shared" si="3"/>
         <v>-0.31635608999999998</v>
       </c>
-      <c r="K24" s="64">
+      <c r="K24" s="55">
         <f t="shared" si="4"/>
         <v>-1.4277649468919265</v>
       </c>
-      <c r="L24" s="69">
+      <c r="L24" s="60">
         <f t="shared" si="5"/>
         <v>0.31635608999999998</v>
       </c>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="74" t="str">
+      <c r="A25" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A25,"-int")</f>
         <v>G5 1/2-int</v>
       </c>
-      <c r="B25" s="68">
+      <c r="B25" s="59">
         <f>'BSPP thread'!C25</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C25" s="101">
+      <c r="C25" s="88">
         <f>'BSPP thread'!$M25/2+5*$B25/(24*TAN(phi/2))*1.05</f>
         <v>75.850026066194843</v>
       </c>
-      <c r="D25" s="76">
+      <c r="D25" s="67">
         <f>'BSPP thread'!$M25+5*$B25/(12*TAN(phi/2))</f>
         <v>151.60764488799018</v>
       </c>
-      <c r="E25" s="68">
+      <c r="E25" s="59">
         <f>'BSPP thread'!$M25/2+5*$B25/(24*TAN(phi/2))*1.05-C25</f>
         <v>0</v>
       </c>
-      <c r="F25" s="64">
+      <c r="F25" s="55">
         <f t="shared" si="0"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="G25" s="64">
+      <c r="G25" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H25" s="64">
+      <c r="H25" s="55">
         <f t="shared" si="2"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="I25" s="64">
+      <c r="I25" s="55">
         <f>'BSPP thread'!$M25/2-$B25*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C25</f>
         <v>-1.4277649468919265</v>
       </c>
-      <c r="J25" s="64">
+      <c r="J25" s="55">
         <f t="shared" si="3"/>
         <v>-0.31635608999999998</v>
       </c>
-      <c r="K25" s="64">
+      <c r="K25" s="55">
         <f t="shared" si="4"/>
         <v>-1.4277649468919265</v>
       </c>
-      <c r="L25" s="69">
+      <c r="L25" s="60">
         <f t="shared" si="5"/>
         <v>0.31635608999999998</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="17" thickBot="1">
-      <c r="A26" s="83" t="str">
+      <c r="A26" s="74" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A26,"-int")</f>
         <v>G6-int</v>
       </c>
-      <c r="B26" s="80">
+      <c r="B26" s="71">
         <f>'BSPP thread'!C26</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C26" s="102">
+      <c r="C26" s="89">
         <f>'BSPP thread'!$M26/2+5*$B26/(24*TAN(phi/2))*1.05</f>
         <v>82.200026066194837</v>
       </c>
-      <c r="D26" s="81">
+      <c r="D26" s="72">
         <f>'BSPP thread'!$M26+5*$B26/(12*TAN(phi/2))</f>
         <v>164.30764488799016</v>
       </c>
-      <c r="E26" s="80">
+      <c r="E26" s="71">
         <f>'BSPP thread'!$M26/2+5*$B26/(24*TAN(phi/2))*1.05-C26</f>
         <v>0</v>
       </c>
-      <c r="F26" s="82">
+      <c r="F26" s="73">
         <f t="shared" si="0"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="G26" s="82">
+      <c r="G26" s="73">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H26" s="82">
+      <c r="H26" s="73">
         <f t="shared" si="2"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="I26" s="82">
+      <c r="I26" s="73">
         <f>'BSPP thread'!$M26/2-$B26*(cinternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C26</f>
         <v>-1.4277649468919265</v>
       </c>
-      <c r="J26" s="82">
+      <c r="J26" s="73">
         <f t="shared" si="3"/>
         <v>-0.31635608999999998</v>
       </c>
-      <c r="K26" s="82">
+      <c r="K26" s="73">
         <f t="shared" si="4"/>
         <v>-1.4277649468919265</v>
       </c>
-      <c r="L26" s="84">
+      <c r="L26" s="75">
         <f t="shared" si="5"/>
         <v>0.31635608999999998</v>
       </c>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="73" t="str">
+      <c r="A27" s="64" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A3,"-ext")</f>
         <v>G1/16-ext</v>
       </c>
-      <c r="B27" s="65">
+      <c r="B27" s="56">
         <f>'BSPP thread'!C3</f>
         <v>0.90700000000000003</v>
       </c>
-      <c r="C27" s="103">
+      <c r="C27" s="90">
         <f>'BSPP thread'!$M3/2-5*$B27/(24*TAN(phi/2))*1.05</f>
         <v>3.2166151398706271</v>
       </c>
-      <c r="D27" s="88">
+      <c r="D27" s="79">
         <f>'BSPP thread'!$M3-5*$B27/(12*TAN(phi/2))</f>
         <v>6.4695288378488138</v>
       </c>
-      <c r="E27" s="85">
+      <c r="E27" s="76">
         <f>'BSPP thread'!$M3/2-5*$B27/(24*TAN(phi/2))*1.05-C27</f>
         <v>0</v>
       </c>
-      <c r="F27" s="66">
+      <c r="F27" s="57">
         <f>-0.46875*$B27</f>
         <v>-0.42515625000000001</v>
       </c>
-      <c r="G27" s="66">
+      <c r="G27" s="57">
         <f>E27</f>
         <v>0</v>
       </c>
-      <c r="H27" s="66">
+      <c r="H27" s="57">
         <f t="shared" ref="H27" si="6">-F27</f>
         <v>0.42515625000000001</v>
       </c>
-      <c r="I27" s="66">
+      <c r="I27" s="57">
         <f>'BSPP thread'!$M3/2+$B27*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C27</f>
         <v>0.57800829101097984</v>
       </c>
-      <c r="J27" s="66">
+      <c r="J27" s="57">
         <f>0.13701*$B27</f>
         <v>0.12426806999999999</v>
       </c>
-      <c r="K27" s="66">
+      <c r="K27" s="57">
         <f>I27</f>
         <v>0.57800829101097984</v>
       </c>
-      <c r="L27" s="67">
+      <c r="L27" s="58">
         <f t="shared" ref="L27" si="7">-J27</f>
         <v>-0.12426806999999999</v>
       </c>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="74" t="str">
+      <c r="A28" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A4,"-ext")</f>
         <v>G1/8-ext</v>
       </c>
-      <c r="B28" s="68">
+      <c r="B28" s="59">
         <f>'BSPP thread'!C4</f>
         <v>0.90700000000000003</v>
       </c>
-      <c r="C28" s="101">
+      <c r="C28" s="88">
         <f>'BSPP thread'!$M4/2-5*$B28/(24*TAN(phi/2))*1.05</f>
         <v>4.2191151398706275</v>
       </c>
-      <c r="D28" s="69">
+      <c r="D28" s="60">
         <f>'BSPP thread'!$M4-5*$B28/(12*TAN(phi/2))</f>
         <v>8.4745288378488137</v>
       </c>
-      <c r="E28" s="86">
+      <c r="E28" s="77">
         <f>'BSPP thread'!$M4/2-5*$B28/(24*TAN(phi/2))*1.05-C28</f>
         <v>0</v>
       </c>
-      <c r="F28" s="64">
+      <c r="F28" s="55">
         <f t="shared" ref="F28:F50" si="8">-0.46875*$B28</f>
         <v>-0.42515625000000001</v>
       </c>
-      <c r="G28" s="64">
+      <c r="G28" s="55">
         <f t="shared" ref="G28:G50" si="9">E28</f>
         <v>0</v>
       </c>
-      <c r="H28" s="64">
+      <c r="H28" s="55">
         <f t="shared" ref="H28:H50" si="10">-F28</f>
         <v>0.42515625000000001</v>
       </c>
-      <c r="I28" s="64">
+      <c r="I28" s="55">
         <f>'BSPP thread'!$M4/2+$B28*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C28</f>
         <v>0.57800829101097939</v>
       </c>
-      <c r="J28" s="64">
+      <c r="J28" s="55">
         <f t="shared" ref="J28:J50" si="11">0.13701*$B28</f>
         <v>0.12426806999999999</v>
       </c>
-      <c r="K28" s="64">
+      <c r="K28" s="55">
         <f t="shared" ref="K28:K50" si="12">I28</f>
         <v>0.57800829101097939</v>
       </c>
-      <c r="L28" s="69">
+      <c r="L28" s="60">
         <f t="shared" ref="L28:L50" si="13">-J28</f>
         <v>-0.12426806999999999</v>
       </c>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="74" t="str">
+      <c r="A29" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A5,"-ext")</f>
         <v>G1/4-ext</v>
       </c>
-      <c r="B29" s="68">
+      <c r="B29" s="59">
         <f>'BSPP thread'!C5</f>
         <v>1.337</v>
       </c>
-      <c r="C29" s="101">
+      <c r="C29" s="88">
         <f>'BSPP thread'!$M5/2-5*$B29/(24*TAN(phi/2))*1.05</f>
         <v>5.6199227585524021</v>
       </c>
-      <c r="D29" s="69">
+      <c r="D29" s="60">
         <f>'BSPP thread'!$M5-5*$B29/(12*TAN(phi/2))</f>
         <v>11.293352873433147</v>
       </c>
-      <c r="E29" s="86">
+      <c r="E29" s="77">
         <f>'BSPP thread'!$M5/2-5*$B29/(24*TAN(phi/2))*1.05-C29</f>
         <v>0</v>
       </c>
-      <c r="F29" s="64">
+      <c r="F29" s="55">
         <f t="shared" si="8"/>
         <v>-0.62671874999999999</v>
       </c>
-      <c r="G29" s="64">
+      <c r="G29" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H29" s="64">
+      <c r="H29" s="55">
         <f t="shared" si="10"/>
         <v>0.62671874999999999</v>
       </c>
-      <c r="I29" s="64">
+      <c r="I29" s="55">
         <f>'BSPP thread'!$M5/2+$B29*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C29</f>
         <v>0.85203647748807043</v>
       </c>
-      <c r="J29" s="64">
+      <c r="J29" s="55">
         <f t="shared" si="11"/>
         <v>0.18318236999999998</v>
       </c>
-      <c r="K29" s="64">
+      <c r="K29" s="55">
         <f t="shared" si="12"/>
         <v>0.85203647748807043</v>
       </c>
-      <c r="L29" s="69">
+      <c r="L29" s="60">
         <f t="shared" si="13"/>
         <v>-0.18318236999999998</v>
       </c>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="74" t="str">
+      <c r="A30" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A6,"-ext")</f>
         <v>G3/8-ext</v>
       </c>
-      <c r="B30" s="68">
+      <c r="B30" s="59">
         <f>'BSPP thread'!C6</f>
         <v>1.337</v>
       </c>
-      <c r="C30" s="101">
+      <c r="C30" s="88">
         <f>'BSPP thread'!$M6/2-5*$B30/(24*TAN(phi/2))*1.05</f>
         <v>7.3724227585524016</v>
       </c>
-      <c r="D30" s="69">
+      <c r="D30" s="60">
         <f>'BSPP thread'!$M6-5*$B30/(12*TAN(phi/2))</f>
         <v>14.798352873433146</v>
       </c>
-      <c r="E30" s="86">
+      <c r="E30" s="77">
         <f>'BSPP thread'!$M6/2-5*$B30/(24*TAN(phi/2))*1.05-C30</f>
         <v>0</v>
       </c>
-      <c r="F30" s="64">
+      <c r="F30" s="55">
         <f t="shared" si="8"/>
         <v>-0.62671874999999999</v>
       </c>
-      <c r="G30" s="64">
+      <c r="G30" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H30" s="64">
+      <c r="H30" s="55">
         <f t="shared" si="10"/>
         <v>0.62671874999999999</v>
       </c>
-      <c r="I30" s="64">
+      <c r="I30" s="55">
         <f>'BSPP thread'!$M6/2+$B30*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C30</f>
         <v>0.85203647748807043</v>
       </c>
-      <c r="J30" s="64">
+      <c r="J30" s="55">
         <f t="shared" si="11"/>
         <v>0.18318236999999998</v>
       </c>
-      <c r="K30" s="64">
+      <c r="K30" s="55">
         <f t="shared" si="12"/>
         <v>0.85203647748807043</v>
       </c>
-      <c r="L30" s="69">
+      <c r="L30" s="60">
         <f t="shared" si="13"/>
         <v>-0.18318236999999998</v>
       </c>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="74" t="str">
+      <c r="A31" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A7,"-ext")</f>
         <v>G1/2-ext</v>
       </c>
-      <c r="B31" s="68">
+      <c r="B31" s="59">
         <f>'BSPP thread'!C7</f>
         <v>1.8140000000000001</v>
       </c>
-      <c r="C31" s="101">
+      <c r="C31" s="88">
         <f>'BSPP thread'!$M7/2-5*$B31/(24*TAN(phi/2))*1.05</f>
         <v>9.1697302797412554</v>
       </c>
-      <c r="D31" s="69">
+      <c r="D31" s="60">
         <f>'BSPP thread'!$M7-5*$B31/(12*TAN(phi/2))</f>
         <v>18.412057675697628</v>
       </c>
-      <c r="E31" s="86">
+      <c r="E31" s="77">
         <f>'BSPP thread'!$M7/2-5*$B31/(24*TAN(phi/2))*1.05-C31</f>
         <v>0</v>
       </c>
-      <c r="F31" s="64">
+      <c r="F31" s="55">
         <f t="shared" si="8"/>
         <v>-0.85031250000000003</v>
       </c>
-      <c r="G31" s="64">
+      <c r="G31" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H31" s="64">
+      <c r="H31" s="55">
         <f t="shared" si="10"/>
         <v>0.85031250000000003</v>
       </c>
-      <c r="I31" s="64">
+      <c r="I31" s="55">
         <f>'BSPP thread'!$M7/2+$B31*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C31</f>
         <v>1.1560165820219588</v>
       </c>
-      <c r="J31" s="64">
+      <c r="J31" s="55">
         <f t="shared" si="11"/>
         <v>0.24853613999999999</v>
       </c>
-      <c r="K31" s="64">
+      <c r="K31" s="55">
         <f t="shared" si="12"/>
         <v>1.1560165820219588</v>
       </c>
-      <c r="L31" s="69">
+      <c r="L31" s="60">
         <f t="shared" si="13"/>
         <v>-0.24853613999999999</v>
       </c>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="74" t="str">
+      <c r="A32" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A8,"-ext")</f>
         <v>G5/8-ext</v>
       </c>
-      <c r="B32" s="68">
+      <c r="B32" s="59">
         <f>'BSPP thread'!C8</f>
         <v>1.8140000000000001</v>
       </c>
-      <c r="C32" s="101">
+      <c r="C32" s="88">
         <f>'BSPP thread'!$M8/2-5*$B32/(24*TAN(phi/2))*1.05</f>
         <v>10.147730279741253</v>
       </c>
-      <c r="D32" s="69">
+      <c r="D32" s="60">
         <f>'BSPP thread'!$M8-5*$B32/(12*TAN(phi/2))</f>
         <v>20.368057675697628</v>
       </c>
-      <c r="E32" s="86">
+      <c r="E32" s="77">
         <f>'BSPP thread'!$M8/2-5*$B32/(24*TAN(phi/2))*1.05-C32</f>
         <v>0</v>
       </c>
-      <c r="F32" s="64">
+      <c r="F32" s="55">
         <f t="shared" si="8"/>
         <v>-0.85031250000000003</v>
       </c>
-      <c r="G32" s="64">
+      <c r="G32" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H32" s="64">
+      <c r="H32" s="55">
         <f t="shared" si="10"/>
         <v>0.85031250000000003</v>
       </c>
-      <c r="I32" s="64">
+      <c r="I32" s="55">
         <f>'BSPP thread'!$M8/2+$B32*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C32</f>
         <v>1.1560165820219606</v>
       </c>
-      <c r="J32" s="64">
+      <c r="J32" s="55">
         <f t="shared" si="11"/>
         <v>0.24853613999999999</v>
       </c>
-      <c r="K32" s="64">
+      <c r="K32" s="55">
         <f t="shared" si="12"/>
         <v>1.1560165820219606</v>
       </c>
-      <c r="L32" s="69">
+      <c r="L32" s="60">
         <f t="shared" si="13"/>
         <v>-0.24853613999999999</v>
       </c>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="74" t="str">
+      <c r="A33" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A9,"-ext")</f>
         <v>G3/4-ext</v>
       </c>
-      <c r="B33" s="68">
+      <c r="B33" s="59">
         <f>'BSPP thread'!C9</f>
         <v>1.8140000000000001</v>
       </c>
-      <c r="C33" s="101">
+      <c r="C33" s="88">
         <f>'BSPP thread'!$M9/2-5*$B33/(24*TAN(phi/2))*1.05</f>
         <v>11.912730279741254</v>
       </c>
-      <c r="D33" s="69">
+      <c r="D33" s="60">
         <f>'BSPP thread'!$M9-5*$B33/(12*TAN(phi/2))</f>
         <v>23.898057675697629</v>
       </c>
-      <c r="E33" s="86">
+      <c r="E33" s="77">
         <f>'BSPP thread'!$M9/2-5*$B33/(24*TAN(phi/2))*1.05-C33</f>
         <v>0</v>
       </c>
-      <c r="F33" s="64">
+      <c r="F33" s="55">
         <f t="shared" si="8"/>
         <v>-0.85031250000000003</v>
       </c>
-      <c r="G33" s="64">
+      <c r="G33" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H33" s="64">
+      <c r="H33" s="55">
         <f t="shared" si="10"/>
         <v>0.85031250000000003</v>
       </c>
-      <c r="I33" s="64">
+      <c r="I33" s="55">
         <f>'BSPP thread'!$M9/2+$B33*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C33</f>
         <v>1.1560165820219606</v>
       </c>
-      <c r="J33" s="64">
+      <c r="J33" s="55">
         <f t="shared" si="11"/>
         <v>0.24853613999999999</v>
       </c>
-      <c r="K33" s="64">
+      <c r="K33" s="55">
         <f t="shared" si="12"/>
         <v>1.1560165820219606</v>
       </c>
-      <c r="L33" s="69">
+      <c r="L33" s="60">
         <f t="shared" si="13"/>
         <v>-0.24853613999999999</v>
       </c>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="74" t="str">
+      <c r="A34" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A10,"-ext")</f>
         <v>G7/8-ext</v>
       </c>
-      <c r="B34" s="68">
+      <c r="B34" s="59">
         <f>'BSPP thread'!C10</f>
         <v>1.8140000000000001</v>
       </c>
-      <c r="C34" s="101">
+      <c r="C34" s="88">
         <f>'BSPP thread'!$M10/2-5*$B34/(24*TAN(phi/2))*1.05</f>
         <v>13.792730279741257</v>
       </c>
-      <c r="D34" s="69">
+      <c r="D34" s="60">
         <f>'BSPP thread'!$M10-5*$B34/(12*TAN(phi/2))</f>
         <v>27.658057675697631</v>
       </c>
-      <c r="E34" s="86">
+      <c r="E34" s="77">
         <f>'BSPP thread'!$M10/2-5*$B34/(24*TAN(phi/2))*1.05-C34</f>
         <v>0</v>
       </c>
-      <c r="F34" s="64">
+      <c r="F34" s="55">
         <f t="shared" si="8"/>
         <v>-0.85031250000000003</v>
       </c>
-      <c r="G34" s="64">
+      <c r="G34" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H34" s="64">
+      <c r="H34" s="55">
         <f t="shared" si="10"/>
         <v>0.85031250000000003</v>
       </c>
-      <c r="I34" s="64">
+      <c r="I34" s="55">
         <f>'BSPP thread'!$M10/2+$B34*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C34</f>
         <v>1.1560165820219588</v>
       </c>
-      <c r="J34" s="64">
+      <c r="J34" s="55">
         <f t="shared" si="11"/>
         <v>0.24853613999999999</v>
       </c>
-      <c r="K34" s="64">
+      <c r="K34" s="55">
         <f t="shared" si="12"/>
         <v>1.1560165820219588</v>
       </c>
-      <c r="L34" s="69">
+      <c r="L34" s="60">
         <f t="shared" si="13"/>
         <v>-0.24853613999999999</v>
       </c>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="74" t="str">
+      <c r="A35" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A11,"-ext")</f>
         <v>G1-ext</v>
       </c>
-      <c r="B35" s="68">
+      <c r="B35" s="59">
         <f>'BSPP thread'!C11</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C35" s="101">
+      <c r="C35" s="88">
         <f>'BSPP thread'!$M11/2-5*$B35/(24*TAN(phi/2))*1.05</f>
         <v>14.959723933805158</v>
       </c>
-      <c r="D35" s="69">
+      <c r="D35" s="60">
         <f>'BSPP thread'!$M11-5*$B35/(12*TAN(phi/2))</f>
         <v>30.011855112009822</v>
       </c>
-      <c r="E35" s="86">
+      <c r="E35" s="77">
         <f>'BSPP thread'!$M11/2-5*$B35/(24*TAN(phi/2))*1.05-C35</f>
         <v>0</v>
       </c>
-      <c r="F35" s="64">
+      <c r="F35" s="55">
         <f t="shared" si="8"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="G35" s="64">
+      <c r="G35" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H35" s="64">
+      <c r="H35" s="55">
         <f t="shared" si="10"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="I35" s="64">
+      <c r="I35" s="55">
         <f>'BSPP thread'!$M11/2+$B35*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C35</f>
         <v>1.4714676338967507</v>
       </c>
-      <c r="J35" s="64">
+      <c r="J35" s="55">
         <f t="shared" si="11"/>
         <v>0.31635608999999998</v>
       </c>
-      <c r="K35" s="64">
+      <c r="K35" s="55">
         <f t="shared" si="12"/>
         <v>1.4714676338967507</v>
       </c>
-      <c r="L35" s="69">
+      <c r="L35" s="60">
         <f t="shared" si="13"/>
         <v>-0.31635608999999998</v>
       </c>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="74" t="str">
+      <c r="A36" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A12,"-ext")</f>
         <v>G1 1/8-ext</v>
       </c>
-      <c r="B36" s="68">
+      <c r="B36" s="59">
         <f>'BSPP thread'!C12</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C36" s="101">
+      <c r="C36" s="88">
         <f>'BSPP thread'!$M12/2-5*$B36/(24*TAN(phi/2))*1.05</f>
         <v>17.28372393380516</v>
       </c>
-      <c r="D36" s="69">
+      <c r="D36" s="60">
         <f>'BSPP thread'!$M12-5*$B36/(12*TAN(phi/2))</f>
         <v>34.659855112009829</v>
       </c>
-      <c r="E36" s="86">
+      <c r="E36" s="77">
         <f>'BSPP thread'!$M12/2-5*$B36/(24*TAN(phi/2))*1.05-C36</f>
         <v>0</v>
       </c>
-      <c r="F36" s="64">
+      <c r="F36" s="55">
         <f t="shared" si="8"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="G36" s="64">
+      <c r="G36" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H36" s="64">
+      <c r="H36" s="55">
         <f t="shared" si="10"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="I36" s="64">
+      <c r="I36" s="55">
         <f>'BSPP thread'!$M12/2+$B36*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C36</f>
         <v>1.4714676338967507</v>
       </c>
-      <c r="J36" s="64">
+      <c r="J36" s="55">
         <f t="shared" si="11"/>
         <v>0.31635608999999998</v>
       </c>
-      <c r="K36" s="64">
+      <c r="K36" s="55">
         <f t="shared" si="12"/>
         <v>1.4714676338967507</v>
       </c>
-      <c r="L36" s="69">
+      <c r="L36" s="60">
         <f t="shared" si="13"/>
         <v>-0.31635608999999998</v>
       </c>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="74" t="str">
+      <c r="A37" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A13,"-ext")</f>
         <v>G1 1/4-ext</v>
       </c>
-      <c r="B37" s="68">
+      <c r="B37" s="59">
         <f>'BSPP thread'!C13</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C37" s="101">
+      <c r="C37" s="88">
         <f>'BSPP thread'!$M13/2-5*$B37/(24*TAN(phi/2))*1.05</f>
         <v>19.290223933805159</v>
       </c>
-      <c r="D37" s="69">
+      <c r="D37" s="60">
         <f>'BSPP thread'!$M13-5*$B37/(12*TAN(phi/2))</f>
         <v>38.672855112009827</v>
       </c>
-      <c r="E37" s="86">
+      <c r="E37" s="77">
         <f>'BSPP thread'!$M13/2-5*$B37/(24*TAN(phi/2))*1.05-C37</f>
         <v>0</v>
       </c>
-      <c r="F37" s="64">
+      <c r="F37" s="55">
         <f t="shared" si="8"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="G37" s="64">
+      <c r="G37" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H37" s="64">
+      <c r="H37" s="55">
         <f t="shared" si="10"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="I37" s="64">
+      <c r="I37" s="55">
         <f>'BSPP thread'!$M13/2+$B37*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C37</f>
         <v>1.4714676338967507</v>
       </c>
-      <c r="J37" s="64">
+      <c r="J37" s="55">
         <f t="shared" si="11"/>
         <v>0.31635608999999998</v>
       </c>
-      <c r="K37" s="64">
+      <c r="K37" s="55">
         <f t="shared" si="12"/>
         <v>1.4714676338967507</v>
       </c>
-      <c r="L37" s="69">
+      <c r="L37" s="60">
         <f t="shared" si="13"/>
         <v>-0.31635608999999998</v>
       </c>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="74" t="str">
+      <c r="A38" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A14,"-ext")</f>
         <v>G1 1/2-ext</v>
       </c>
-      <c r="B38" s="68">
+      <c r="B38" s="59">
         <f>'BSPP thread'!C14</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C38" s="101">
+      <c r="C38" s="88">
         <f>'BSPP thread'!$M14/2-5*$B38/(24*TAN(phi/2))*1.05</f>
         <v>22.236723933805159</v>
       </c>
-      <c r="D38" s="69">
+      <c r="D38" s="60">
         <f>'BSPP thread'!$M14-5*$B38/(12*TAN(phi/2))</f>
         <v>44.565855112009828</v>
       </c>
-      <c r="E38" s="86">
+      <c r="E38" s="77">
         <f>'BSPP thread'!$M14/2-5*$B38/(24*TAN(phi/2))*1.05-C38</f>
         <v>0</v>
       </c>
-      <c r="F38" s="64">
+      <c r="F38" s="55">
         <f t="shared" si="8"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="G38" s="64">
+      <c r="G38" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H38" s="64">
+      <c r="H38" s="55">
         <f t="shared" si="10"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="I38" s="64">
+      <c r="I38" s="55">
         <f>'BSPP thread'!$M14/2+$B38*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C38</f>
         <v>1.4714676338967507</v>
       </c>
-      <c r="J38" s="64">
+      <c r="J38" s="55">
         <f t="shared" si="11"/>
         <v>0.31635608999999998</v>
       </c>
-      <c r="K38" s="64">
+      <c r="K38" s="55">
         <f t="shared" si="12"/>
         <v>1.4714676338967507</v>
       </c>
-      <c r="L38" s="69">
+      <c r="L38" s="60">
         <f t="shared" si="13"/>
         <v>-0.31635608999999998</v>
       </c>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="74" t="str">
+      <c r="A39" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A15,"-ext")</f>
         <v>G1 3/4-ext</v>
       </c>
-      <c r="B39" s="68">
+      <c r="B39" s="59">
         <f>'BSPP thread'!C15</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C39" s="101">
+      <c r="C39" s="88">
         <f>'BSPP thread'!$M15/2-5*$B39/(24*TAN(phi/2))*1.05</f>
         <v>25.208223933805161</v>
       </c>
-      <c r="D39" s="69">
+      <c r="D39" s="60">
         <f>'BSPP thread'!$M15-5*$B39/(12*TAN(phi/2))</f>
         <v>50.508855112009833</v>
       </c>
-      <c r="E39" s="86">
+      <c r="E39" s="77">
         <f>'BSPP thread'!$M15/2-5*$B39/(24*TAN(phi/2))*1.05-C39</f>
         <v>0</v>
       </c>
-      <c r="F39" s="64">
+      <c r="F39" s="55">
         <f t="shared" si="8"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="G39" s="64">
+      <c r="G39" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H39" s="64">
+      <c r="H39" s="55">
         <f t="shared" si="10"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="I39" s="64">
+      <c r="I39" s="55">
         <f>'BSPP thread'!$M15/2+$B39*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C39</f>
         <v>1.4714676338967507</v>
       </c>
-      <c r="J39" s="64">
+      <c r="J39" s="55">
         <f t="shared" si="11"/>
         <v>0.31635608999999998</v>
       </c>
-      <c r="K39" s="64">
+      <c r="K39" s="55">
         <f t="shared" si="12"/>
         <v>1.4714676338967507</v>
       </c>
-      <c r="L39" s="69">
+      <c r="L39" s="60">
         <f t="shared" si="13"/>
         <v>-0.31635608999999998</v>
       </c>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="74" t="str">
+      <c r="A40" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A16,"-ext")</f>
         <v>G2-ext</v>
       </c>
-      <c r="B40" s="68">
+      <c r="B40" s="59">
         <f>'BSPP thread'!C16</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C40" s="101">
+      <c r="C40" s="88">
         <f>'BSPP thread'!$M16/2-5*$B40/(24*TAN(phi/2))*1.05</f>
         <v>28.142223933805159</v>
       </c>
-      <c r="D40" s="69">
+      <c r="D40" s="60">
         <f>'BSPP thread'!$M16-5*$B40/(12*TAN(phi/2))</f>
         <v>56.376855112009828</v>
       </c>
-      <c r="E40" s="86">
+      <c r="E40" s="77">
         <f>'BSPP thread'!$M16/2-5*$B40/(24*TAN(phi/2))*1.05-C40</f>
         <v>0</v>
       </c>
-      <c r="F40" s="64">
+      <c r="F40" s="55">
         <f t="shared" si="8"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="G40" s="64">
+      <c r="G40" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H40" s="64">
+      <c r="H40" s="55">
         <f t="shared" si="10"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="I40" s="64">
+      <c r="I40" s="55">
         <f>'BSPP thread'!$M16/2+$B40*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C40</f>
         <v>1.4714676338967507</v>
       </c>
-      <c r="J40" s="64">
+      <c r="J40" s="55">
         <f t="shared" si="11"/>
         <v>0.31635608999999998</v>
       </c>
-      <c r="K40" s="64">
+      <c r="K40" s="55">
         <f t="shared" si="12"/>
         <v>1.4714676338967507</v>
       </c>
-      <c r="L40" s="69">
+      <c r="L40" s="60">
         <f t="shared" si="13"/>
         <v>-0.31635608999999998</v>
       </c>
     </row>
     <row r="41" spans="1:12">
-      <c r="A41" s="74" t="str">
+      <c r="A41" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A17,"-ext")</f>
         <v>G2 1/4-ext</v>
       </c>
-      <c r="B41" s="68">
+      <c r="B41" s="59">
         <f>'BSPP thread'!C17</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C41" s="101">
+      <c r="C41" s="88">
         <f>'BSPP thread'!$M17/2-5*$B41/(24*TAN(phi/2))*1.05</f>
         <v>31.199473933805159</v>
       </c>
-      <c r="D41" s="69">
+      <c r="D41" s="60">
         <f>'BSPP thread'!$M17-5*$B41/(12*TAN(phi/2))</f>
         <v>62.491355112009828</v>
       </c>
-      <c r="E41" s="86">
+      <c r="E41" s="77">
         <f>'BSPP thread'!$M17/2-5*$B41/(24*TAN(phi/2))*1.05-C41</f>
         <v>0</v>
       </c>
-      <c r="F41" s="64">
+      <c r="F41" s="55">
         <f t="shared" si="8"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="G41" s="64">
+      <c r="G41" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H41" s="64">
+      <c r="H41" s="55">
         <f t="shared" si="10"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="I41" s="64">
+      <c r="I41" s="55">
         <f>'BSPP thread'!$M17/2+$B41*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C41</f>
         <v>1.4714676338967507</v>
       </c>
-      <c r="J41" s="64">
+      <c r="J41" s="55">
         <f t="shared" si="11"/>
         <v>0.31635608999999998</v>
       </c>
-      <c r="K41" s="64">
+      <c r="K41" s="55">
         <f t="shared" si="12"/>
         <v>1.4714676338967507</v>
       </c>
-      <c r="L41" s="69">
+      <c r="L41" s="60">
         <f t="shared" si="13"/>
         <v>-0.31635608999999998</v>
       </c>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="74" t="str">
+      <c r="A42" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A18,"-ext")</f>
         <v>G2 1/2-ext</v>
       </c>
-      <c r="B42" s="68">
+      <c r="B42" s="59">
         <f>'BSPP thread'!C18</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C42" s="101">
+      <c r="C42" s="88">
         <f>'BSPP thread'!$M18/2-5*$B42/(24*TAN(phi/2))*1.05</f>
         <v>35.936473933805161</v>
       </c>
-      <c r="D42" s="69">
+      <c r="D42" s="60">
         <f>'BSPP thread'!$M18-5*$B42/(12*TAN(phi/2))</f>
         <v>71.965355112009831</v>
       </c>
-      <c r="E42" s="86">
+      <c r="E42" s="77">
         <f>'BSPP thread'!$M18/2-5*$B42/(24*TAN(phi/2))*1.05-C42</f>
         <v>0</v>
       </c>
-      <c r="F42" s="64">
+      <c r="F42" s="55">
         <f t="shared" si="8"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="G42" s="64">
+      <c r="G42" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H42" s="64">
+      <c r="H42" s="55">
         <f t="shared" si="10"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="I42" s="64">
+      <c r="I42" s="55">
         <f>'BSPP thread'!$M18/2+$B42*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C42</f>
         <v>1.4714676338967507</v>
       </c>
-      <c r="J42" s="64">
+      <c r="J42" s="55">
         <f t="shared" si="11"/>
         <v>0.31635608999999998</v>
       </c>
-      <c r="K42" s="64">
+      <c r="K42" s="55">
         <f t="shared" si="12"/>
         <v>1.4714676338967507</v>
       </c>
-      <c r="L42" s="69">
+      <c r="L42" s="60">
         <f t="shared" si="13"/>
         <v>-0.31635608999999998</v>
       </c>
     </row>
     <row r="43" spans="1:12">
-      <c r="A43" s="74" t="str">
+      <c r="A43" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A19,"-ext")</f>
         <v>G2 3/4-ext</v>
       </c>
-      <c r="B43" s="68">
+      <c r="B43" s="59">
         <f>'BSPP thread'!C19</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C43" s="101">
+      <c r="C43" s="88">
         <f>'BSPP thread'!$M19/2-5*$B43/(24*TAN(phi/2))*1.05</f>
         <v>39.111473933805165</v>
       </c>
-      <c r="D43" s="69">
+      <c r="D43" s="60">
         <f>'BSPP thread'!$M19-5*$B43/(12*TAN(phi/2))</f>
         <v>78.31535511200984</v>
       </c>
-      <c r="E43" s="86">
+      <c r="E43" s="77">
         <f>'BSPP thread'!$M19/2-5*$B43/(24*TAN(phi/2))*1.05-C43</f>
         <v>0</v>
       </c>
-      <c r="F43" s="64">
+      <c r="F43" s="55">
         <f t="shared" si="8"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="G43" s="64">
+      <c r="G43" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H43" s="64">
+      <c r="H43" s="55">
         <f t="shared" si="10"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="I43" s="64">
+      <c r="I43" s="55">
         <f>'BSPP thread'!$M19/2+$B43*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C43</f>
         <v>1.4714676338967507</v>
       </c>
-      <c r="J43" s="64">
+      <c r="J43" s="55">
         <f t="shared" si="11"/>
         <v>0.31635608999999998</v>
       </c>
-      <c r="K43" s="64">
+      <c r="K43" s="55">
         <f t="shared" si="12"/>
         <v>1.4714676338967507</v>
       </c>
-      <c r="L43" s="69">
+      <c r="L43" s="60">
         <f t="shared" si="13"/>
         <v>-0.31635608999999998</v>
       </c>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="74" t="str">
+      <c r="A44" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A20,"-ext")</f>
         <v>G3-ext</v>
       </c>
-      <c r="B44" s="68">
+      <c r="B44" s="59">
         <f>'BSPP thread'!C20</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C44" s="101">
+      <c r="C44" s="88">
         <f>'BSPP thread'!$M20/2-5*$B44/(24*TAN(phi/2))*1.05</f>
         <v>42.286473933805162</v>
       </c>
-      <c r="D44" s="69">
+      <c r="D44" s="60">
         <f>'BSPP thread'!$M20-5*$B44/(12*TAN(phi/2))</f>
         <v>84.665355112009834</v>
       </c>
-      <c r="E44" s="86">
+      <c r="E44" s="77">
         <f>'BSPP thread'!$M20/2-5*$B44/(24*TAN(phi/2))*1.05-C44</f>
         <v>0</v>
       </c>
-      <c r="F44" s="64">
+      <c r="F44" s="55">
         <f t="shared" si="8"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="G44" s="64">
+      <c r="G44" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H44" s="64">
+      <c r="H44" s="55">
         <f t="shared" si="10"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="I44" s="64">
+      <c r="I44" s="55">
         <f>'BSPP thread'!$M20/2+$B44*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C44</f>
         <v>1.4714676338967507</v>
       </c>
-      <c r="J44" s="64">
+      <c r="J44" s="55">
         <f t="shared" si="11"/>
         <v>0.31635608999999998</v>
       </c>
-      <c r="K44" s="64">
+      <c r="K44" s="55">
         <f t="shared" si="12"/>
         <v>1.4714676338967507</v>
       </c>
-      <c r="L44" s="69">
+      <c r="L44" s="60">
         <f t="shared" si="13"/>
         <v>-0.31635608999999998</v>
       </c>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="74" t="str">
+      <c r="A45" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A21,"-ext")</f>
         <v>G3 1/2-ext</v>
       </c>
-      <c r="B45" s="68">
+      <c r="B45" s="59">
         <f>'BSPP thread'!C21</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C45" s="101">
+      <c r="C45" s="88">
         <f>'BSPP thread'!$M21/2-5*$B45/(24*TAN(phi/2))*1.05</f>
         <v>48.509473933805161</v>
       </c>
-      <c r="D45" s="69">
+      <c r="D45" s="60">
         <f>'BSPP thread'!$M21-5*$B45/(12*TAN(phi/2))</f>
         <v>97.111355112009832</v>
       </c>
-      <c r="E45" s="86">
+      <c r="E45" s="77">
         <f>'BSPP thread'!$M21/2-5*$B45/(24*TAN(phi/2))*1.05-C45</f>
         <v>0</v>
       </c>
-      <c r="F45" s="64">
+      <c r="F45" s="55">
         <f t="shared" si="8"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="G45" s="64">
+      <c r="G45" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H45" s="64">
+      <c r="H45" s="55">
         <f t="shared" si="10"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="I45" s="64">
+      <c r="I45" s="55">
         <f>'BSPP thread'!$M21/2+$B45*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C45</f>
         <v>1.4714676338967507</v>
       </c>
-      <c r="J45" s="64">
+      <c r="J45" s="55">
         <f t="shared" si="11"/>
         <v>0.31635608999999998</v>
       </c>
-      <c r="K45" s="64">
+      <c r="K45" s="55">
         <f t="shared" si="12"/>
         <v>1.4714676338967507</v>
       </c>
-      <c r="L45" s="69">
+      <c r="L45" s="60">
         <f t="shared" si="13"/>
         <v>-0.31635608999999998</v>
       </c>
     </row>
     <row r="46" spans="1:12">
-      <c r="A46" s="74" t="str">
+      <c r="A46" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A22,"-ext")</f>
         <v>G4-ext</v>
       </c>
-      <c r="B46" s="68">
+      <c r="B46" s="59">
         <f>'BSPP thread'!C22</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C46" s="101">
+      <c r="C46" s="88">
         <f>'BSPP thread'!$M22/2-5*$B46/(24*TAN(phi/2))*1.05</f>
         <v>54.859473933805162</v>
       </c>
-      <c r="D46" s="69">
+      <c r="D46" s="60">
         <f>'BSPP thread'!$M22-5*$B46/(12*TAN(phi/2))</f>
         <v>109.81135511200984</v>
       </c>
-      <c r="E46" s="86">
+      <c r="E46" s="77">
         <f>'BSPP thread'!$M22/2-5*$B46/(24*TAN(phi/2))*1.05-C46</f>
         <v>0</v>
       </c>
-      <c r="F46" s="64">
+      <c r="F46" s="55">
         <f t="shared" si="8"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="G46" s="64">
+      <c r="G46" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H46" s="64">
+      <c r="H46" s="55">
         <f t="shared" si="10"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="I46" s="64">
+      <c r="I46" s="55">
         <f>'BSPP thread'!$M22/2+$B46*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C46</f>
         <v>1.4714676338967507</v>
       </c>
-      <c r="J46" s="64">
+      <c r="J46" s="55">
         <f t="shared" si="11"/>
         <v>0.31635608999999998</v>
       </c>
-      <c r="K46" s="64">
+      <c r="K46" s="55">
         <f t="shared" si="12"/>
         <v>1.4714676338967507</v>
       </c>
-      <c r="L46" s="69">
+      <c r="L46" s="60">
         <f t="shared" si="13"/>
         <v>-0.31635608999999998</v>
       </c>
     </row>
     <row r="47" spans="1:12">
-      <c r="A47" s="74" t="str">
+      <c r="A47" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A23,"-ext")</f>
         <v>G4 1/2-ext</v>
       </c>
-      <c r="B47" s="68">
+      <c r="B47" s="59">
         <f>'BSPP thread'!C23</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C47" s="101">
+      <c r="C47" s="88">
         <f>'BSPP thread'!$M23/2-5*$B47/(24*TAN(phi/2))*1.05</f>
         <v>61.209473933805164</v>
       </c>
-      <c r="D47" s="69">
+      <c r="D47" s="60">
         <f>'BSPP thread'!$M23-5*$B47/(12*TAN(phi/2))</f>
         <v>122.51135511200984</v>
       </c>
-      <c r="E47" s="86">
+      <c r="E47" s="77">
         <f>'BSPP thread'!$M23/2-5*$B47/(24*TAN(phi/2))*1.05-C47</f>
         <v>0</v>
       </c>
-      <c r="F47" s="64">
+      <c r="F47" s="55">
         <f t="shared" si="8"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="G47" s="64">
+      <c r="G47" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H47" s="64">
+      <c r="H47" s="55">
         <f t="shared" si="10"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="I47" s="64">
+      <c r="I47" s="55">
         <f>'BSPP thread'!$M23/2+$B47*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C47</f>
         <v>1.4714676338967507</v>
       </c>
-      <c r="J47" s="64">
+      <c r="J47" s="55">
         <f t="shared" si="11"/>
         <v>0.31635608999999998</v>
       </c>
-      <c r="K47" s="64">
+      <c r="K47" s="55">
         <f t="shared" si="12"/>
         <v>1.4714676338967507</v>
       </c>
-      <c r="L47" s="69">
+      <c r="L47" s="60">
         <f t="shared" si="13"/>
         <v>-0.31635608999999998</v>
       </c>
     </row>
     <row r="48" spans="1:12">
-      <c r="A48" s="74" t="str">
+      <c r="A48" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A24,"-ext")</f>
         <v>G5-ext</v>
       </c>
-      <c r="B48" s="68">
+      <c r="B48" s="59">
         <f>'BSPP thread'!C24</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C48" s="101">
+      <c r="C48" s="88">
         <f>'BSPP thread'!$M24/2-5*$B48/(24*TAN(phi/2))*1.05</f>
         <v>67.559473933805151</v>
       </c>
-      <c r="D48" s="69">
+      <c r="D48" s="60">
         <f>'BSPP thread'!$M24-5*$B48/(12*TAN(phi/2))</f>
         <v>135.21135511200981</v>
       </c>
-      <c r="E48" s="86">
+      <c r="E48" s="77">
         <f>'BSPP thread'!$M24/2-5*$B48/(24*TAN(phi/2))*1.05-C48</f>
         <v>0</v>
       </c>
-      <c r="F48" s="64">
+      <c r="F48" s="55">
         <f t="shared" si="8"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="G48" s="64">
+      <c r="G48" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H48" s="64">
+      <c r="H48" s="55">
         <f t="shared" si="10"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="I48" s="64">
+      <c r="I48" s="55">
         <f>'BSPP thread'!$M24/2+$B48*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C48</f>
         <v>1.4714676338967507</v>
       </c>
-      <c r="J48" s="64">
+      <c r="J48" s="55">
         <f t="shared" si="11"/>
         <v>0.31635608999999998</v>
       </c>
-      <c r="K48" s="64">
+      <c r="K48" s="55">
         <f t="shared" si="12"/>
         <v>1.4714676338967507</v>
       </c>
-      <c r="L48" s="69">
+      <c r="L48" s="60">
         <f t="shared" si="13"/>
         <v>-0.31635608999999998</v>
       </c>
     </row>
     <row r="49" spans="1:12">
-      <c r="A49" s="74" t="str">
+      <c r="A49" s="65" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A25,"-ext")</f>
         <v>G5 1/2-ext</v>
       </c>
-      <c r="B49" s="68">
+      <c r="B49" s="59">
         <f>'BSPP thread'!C25</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C49" s="101">
+      <c r="C49" s="88">
         <f>'BSPP thread'!$M25/2-5*$B49/(24*TAN(phi/2))*1.05</f>
         <v>73.90947393380516</v>
       </c>
-      <c r="D49" s="69">
+      <c r="D49" s="60">
         <f>'BSPP thread'!$M25-5*$B49/(12*TAN(phi/2))</f>
         <v>147.91135511200983</v>
       </c>
-      <c r="E49" s="86">
+      <c r="E49" s="77">
         <f>'BSPP thread'!$M25/2-5*$B49/(24*TAN(phi/2))*1.05-C49</f>
         <v>0</v>
       </c>
-      <c r="F49" s="64">
+      <c r="F49" s="55">
         <f t="shared" si="8"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="G49" s="64">
+      <c r="G49" s="55">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H49" s="64">
+      <c r="H49" s="55">
         <f t="shared" si="10"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="I49" s="64">
+      <c r="I49" s="55">
         <f>'BSPP thread'!$M25/2+$B49*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C49</f>
         <v>1.4714676338967507</v>
       </c>
-      <c r="J49" s="64">
+      <c r="J49" s="55">
         <f t="shared" si="11"/>
         <v>0.31635608999999998</v>
       </c>
-      <c r="K49" s="64">
+      <c r="K49" s="55">
         <f t="shared" si="12"/>
         <v>1.4714676338967507</v>
       </c>
-      <c r="L49" s="69">
+      <c r="L49" s="60">
         <f t="shared" si="13"/>
         <v>-0.31635608999999998</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="17" thickBot="1">
-      <c r="A50" s="75" t="str">
+      <c r="A50" s="66" t="str">
         <f>_xlfn.CONCAT("G",'BSPP thread'!A26,"-ext")</f>
         <v>G6-ext</v>
       </c>
-      <c r="B50" s="70">
+      <c r="B50" s="61">
         <f>'BSPP thread'!C26</f>
         <v>2.3090000000000002</v>
       </c>
-      <c r="C50" s="104">
+      <c r="C50" s="91">
         <f>'BSPP thread'!$M26/2-5*$B50/(24*TAN(phi/2))*1.05</f>
         <v>80.259473933805154</v>
       </c>
-      <c r="D50" s="72">
+      <c r="D50" s="63">
         <f>'BSPP thread'!$M26-5*$B50/(12*TAN(phi/2))</f>
         <v>160.61135511200982</v>
       </c>
-      <c r="E50" s="87">
+      <c r="E50" s="78">
         <f>'BSPP thread'!$M26/2-5*$B50/(24*TAN(phi/2))*1.05-C50</f>
         <v>0</v>
       </c>
-      <c r="F50" s="71">
+      <c r="F50" s="62">
         <f t="shared" si="8"/>
         <v>-1.0823437500000002</v>
       </c>
-      <c r="G50" s="71">
+      <c r="G50" s="62">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H50" s="71">
+      <c r="H50" s="62">
         <f t="shared" si="10"/>
         <v>1.0823437500000002</v>
       </c>
-      <c r="I50" s="71">
+      <c r="I50" s="62">
         <f>'BSPP thread'!$M26/2+$B50*(cexternal-TAN((PI()+phi)/4)/12*(1-SIN(phi/2)))-C50</f>
         <v>1.4714676338967507</v>
       </c>
-      <c r="J50" s="71">
+      <c r="J50" s="62">
         <f t="shared" si="11"/>
         <v>0.31635608999999998</v>
       </c>
-      <c r="K50" s="71">
+      <c r="K50" s="62">
         <f t="shared" si="12"/>
         <v>1.4714676338967507</v>
       </c>
-      <c r="L50" s="72">
+      <c r="L50" s="63">
         <f t="shared" si="13"/>
         <v>-0.31635608999999998</v>
       </c>

</xml_diff>